<commit_message>
commit with export button on drug page
</commit_message>
<xml_diff>
--- a/actioncard_listt.xlsx
+++ b/actioncard_listt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Index</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>action card 3</t>
+  </si>
+  <si>
+    <t>action card 4</t>
+  </si>
+  <si>
+    <t>action card 5</t>
   </si>
 </sst>
 </file>
@@ -522,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B49"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -897,6 +903,30 @@
         <v>44</v>
       </c>
     </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
commit with import export operation on actioncard wth documentation
</commit_message>
<xml_diff>
--- a/actioncard_listt.xlsx
+++ b/actioncard_listt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Index</t>
   </si>
@@ -136,22 +136,16 @@
     <t>Definition and complications</t>
   </si>
   <si>
-    <t>New action card</t>
-  </si>
-  <si>
-    <t>action card 1</t>
-  </si>
-  <si>
-    <t>action card 2</t>
-  </si>
-  <si>
-    <t>action card 3</t>
-  </si>
-  <si>
-    <t>action card 4</t>
-  </si>
-  <si>
     <t>action card 5</t>
+  </si>
+  <si>
+    <t>Emotinal health</t>
+  </si>
+  <si>
+    <t>Happyness</t>
+  </si>
+  <si>
+    <t>safe-delivery</t>
   </si>
 </sst>
 </file>
@@ -528,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B44"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -868,7 +862,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -876,7 +870,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -884,47 +878,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
         <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>